<commit_message>
Updated figures, data, station coordinates.
</commit_message>
<xml_diff>
--- a/Data/zoop_stations.xlsx
+++ b/Data/zoop_stations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Zooplankton synthesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\Water-conditions-report\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1779,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G381"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A325" workbookViewId="0">
+      <selection activeCell="D344" sqref="D344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6492,7 +6492,7 @@
         <v>38.008040000000001</v>
       </c>
       <c r="D343" s="30">
-        <v>-21.456099999999999</v>
+        <v>-121.45610000000001</v>
       </c>
     </row>
     <row r="344" spans="1:4">

</xml_diff>